<commit_message>
fixed minor usb protocol issues
</commit_message>
<xml_diff>
--- a/Docs/Function list.xlsx
+++ b/Docs/Function list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\joaov\Documents\Poli\PANDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\joaov\Documents\Poli\PANDA\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4A69AF-5452-459E-8AD1-CEE1486B2577}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9AB158-8EC5-4759-B6D0-09BE64DF1422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{8C328E55-AF09-4F7F-81D1-A402C4DF80EF}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="9072" xr2:uid="{8C328E55-AF09-4F7F-81D1-A402C4DF80EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>Request functions</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>SetUsbActive</t>
+  </si>
+  <si>
+    <t>GetUsbActive</t>
   </si>
 </sst>
 </file>
@@ -202,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -210,6 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC713BAC-C8AB-4C8D-A255-A5F2FC904122}">
   <dimension ref="A2:H138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,7 +628,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="E9">
         <f t="shared" si="1"/>
         <v>133</v>
@@ -632,7 +641,9 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="E10">
         <f t="shared" si="1"/>
         <v>134</v>

</xml_diff>